<commit_message>
add fail page for wrong answered attention checks
</commit_message>
<xml_diff>
--- a/_static/data/traffic_data.xlsx
+++ b/_static/data/traffic_data.xlsx
@@ -88,7 +88,7 @@
     <t xml:space="preserve">Motorcycle</t>
   </si>
   <si>
-    <t xml:space="preserve">canceled </t>
+    <t xml:space="preserve">Canceled </t>
   </si>
   <si>
     <t xml:space="preserve">83 min</t>
@@ -466,17 +466,17 @@
   </sheetPr>
   <dimension ref="A1:D50"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="I17" activeCellId="0" sqref="I17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="7.30078125" defaultRowHeight="19.9" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="6.37890625" defaultRowHeight="19.9" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="8.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="15.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="6.87"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="5" style="1" width="7.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="14.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="12.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="13.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="7.76"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="5" style="1" width="6.38"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="27.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>